<commit_message>
restructure code and remove unused features
</commit_message>
<xml_diff>
--- a/input_data/impact_functions/annual_deaths.xlsx
+++ b/input_data/impact_functions/annual_deaths.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliestalhanske/python_projects/master_thesis-master/input_data/impact_functions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliestalhanske/python_projects/heat_mortality_impact/input_data/impact_functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418D90BC-2FF0-2341-8941-E98B82245065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A21EB70-7BD1-134D-A926-AD7A264C7E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="19200" windowHeight="7060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="19200" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="u75" sheetId="1" r:id="rId1"/>
-    <sheet name="o75" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="34">
   <si>
     <t>Aargau</t>
   </si>
@@ -120,23 +119,39 @@
     <t>%</t>
   </si>
   <si>
-    <t>Canton</t>
-  </si>
-  <si>
-    <t>Annual_deaths</t>
-  </si>
-  <si>
     <t>CH</t>
+  </si>
+  <si>
+    <t>canton</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>annual_deaths</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -169,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -181,9 +196,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -474,397 +486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="4">
-        <f>D2*C$2</f>
-        <v>18247.936000000002</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="D2" s="3">
-        <v>67088</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4">
-        <f t="shared" ref="B3:B28" si="0">D3*C$2</f>
-        <v>1300.1600000000001</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
-        <v>4780</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4">
-        <f t="shared" si="0"/>
-        <v>124.84800000000001</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4">
-        <f t="shared" si="0"/>
-        <v>37.264000000000003</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
-        <v>665.31200000000001</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <v>2446</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
-        <v>564.94400000000007</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
-        <v>2077</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
-        <v>2570.672</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <v>9451</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
-        <v>559.77600000000007</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
-        <v>2058</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
-        <v>920.72</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3">
-        <v>3385</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
-        <v>98.736000000000004</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4">
-        <f t="shared" si="0"/>
-        <v>486.60800000000006</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4">
-        <f t="shared" si="0"/>
-        <v>184.96</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
-        <f t="shared" si="0"/>
-        <v>854.08</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
-        <v>3140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4">
-        <f t="shared" si="0"/>
-        <v>435.47200000000004</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
-        <v>1601</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4">
-        <f t="shared" si="0"/>
-        <v>81.872</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4">
-        <f t="shared" si="0"/>
-        <v>70.176000000000002</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4">
-        <f t="shared" si="0"/>
-        <v>210.52800000000002</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4">
-        <f t="shared" si="0"/>
-        <v>313.34400000000005</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4">
-        <f t="shared" si="0"/>
-        <v>670.20800000000008</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3">
-        <v>2464</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4">
-        <f t="shared" si="0"/>
-        <v>1055.3600000000001</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
-        <v>3880</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4">
-        <f t="shared" si="0"/>
-        <v>562.22400000000005</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
-        <v>2067</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="4">
-        <f t="shared" si="0"/>
-        <v>857.34400000000005</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3">
-        <v>3152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4">
-        <f t="shared" si="0"/>
-        <v>88.128</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="4">
-        <f t="shared" si="0"/>
-        <v>740.928</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3">
-        <v>2724</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="shared" si="0"/>
-        <v>1564</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3">
-        <v>5750</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4">
-        <f t="shared" si="0"/>
-        <v>221.40800000000002</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="4">
-        <f t="shared" si="0"/>
-        <v>3008.864</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3">
-        <v>11062</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -873,36 +499,42 @@
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2">
         <f>D2*C$2</f>
         <v>48840.063999999998</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>0.72799999999999998</v>
       </c>
       <c r="D2" s="3">
         <v>67088</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -914,8 +546,11 @@
       <c r="D3" s="3">
         <v>4780</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -927,8 +562,11 @@
       <c r="D4" s="3">
         <v>459</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -940,8 +578,11 @@
       <c r="D5" s="3">
         <v>137</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -953,8 +594,11 @@
       <c r="D6" s="3">
         <v>2446</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -966,8 +610,11 @@
       <c r="D7" s="3">
         <v>2077</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -979,8 +626,11 @@
       <c r="D8" s="3">
         <v>9451</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -992,8 +642,11 @@
       <c r="D9" s="3">
         <v>2058</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1005,8 +658,11 @@
       <c r="D10" s="3">
         <v>3385</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1018,8 +674,11 @@
       <c r="D11" s="3">
         <v>363</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1031,8 +690,11 @@
       <c r="D12" s="3">
         <v>1789</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1044,8 +706,11 @@
       <c r="D13" s="3">
         <v>680</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1057,8 +722,11 @@
       <c r="D14" s="3">
         <v>3140</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1070,8 +738,11 @@
       <c r="D15" s="3">
         <v>1601</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1083,8 +754,11 @@
       <c r="D16" s="3">
         <v>301</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1096,8 +770,11 @@
       <c r="D17" s="3">
         <v>258</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1109,8 +786,11 @@
       <c r="D18" s="3">
         <v>774</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1122,8 +802,11 @@
       <c r="D19" s="3">
         <v>1152</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1135,8 +818,11 @@
       <c r="D20" s="3">
         <v>2464</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1148,8 +834,11 @@
       <c r="D21" s="3">
         <v>3880</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1161,8 +850,11 @@
       <c r="D22" s="3">
         <v>2067</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1174,8 +866,11 @@
       <c r="D23" s="3">
         <v>3152</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1187,8 +882,11 @@
       <c r="D24" s="3">
         <v>324</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1200,8 +898,11 @@
       <c r="D25" s="3">
         <v>2724</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1213,8 +914,11 @@
       <c r="D26" s="3">
         <v>5750</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1226,8 +930,11 @@
       <c r="D27" s="3">
         <v>814</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1239,8 +946,446 @@
       <c r="D28" s="3">
         <v>11062</v>
       </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4">
+        <f>D29*C$29</f>
+        <v>18247.936000000002</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="D29" s="3">
+        <v>67088</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:B55" si="1">D30*C$29</f>
+        <v>1300.1600000000001</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <v>4780</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="1"/>
+        <v>124.84800000000001</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3">
+        <v>459</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="1"/>
+        <v>37.264000000000003</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3">
+        <v>137</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="1"/>
+        <v>665.31200000000001</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3">
+        <v>2446</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="1"/>
+        <v>564.94400000000007</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3">
+        <v>2077</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="1"/>
+        <v>2570.672</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3">
+        <v>9451</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="1"/>
+        <v>559.77600000000007</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3">
+        <v>2058</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" si="1"/>
+        <v>920.72</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3">
+        <v>3385</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" si="1"/>
+        <v>98.736000000000004</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <v>363</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="4">
+        <f t="shared" si="1"/>
+        <v>486.60800000000006</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3">
+        <v>1789</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4">
+        <f t="shared" si="1"/>
+        <v>184.96</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3">
+        <v>680</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="4">
+        <f t="shared" si="1"/>
+        <v>854.08</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3">
+        <v>3140</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="4">
+        <f t="shared" si="1"/>
+        <v>435.47200000000004</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3">
+        <v>1601</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="4">
+        <f t="shared" si="1"/>
+        <v>81.872</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3">
+        <v>301</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="4">
+        <f t="shared" si="1"/>
+        <v>70.176000000000002</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3">
+        <v>258</v>
+      </c>
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="4">
+        <f t="shared" si="1"/>
+        <v>210.52800000000002</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3">
+        <v>774</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="4">
+        <f t="shared" si="1"/>
+        <v>313.34400000000005</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3">
+        <v>1152</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="4">
+        <f t="shared" si="1"/>
+        <v>670.20800000000008</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3">
+        <v>2464</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="4">
+        <f t="shared" si="1"/>
+        <v>1055.3600000000001</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3">
+        <v>3880</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="4">
+        <f t="shared" si="1"/>
+        <v>562.22400000000005</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3">
+        <v>2067</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="4">
+        <f t="shared" si="1"/>
+        <v>857.34400000000005</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3">
+        <v>3152</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="4">
+        <f t="shared" si="1"/>
+        <v>88.128</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3">
+        <v>324</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="4">
+        <f t="shared" si="1"/>
+        <v>740.928</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3">
+        <v>2724</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="4">
+        <f t="shared" si="1"/>
+        <v>1564</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3">
+        <v>5750</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="4">
+        <f t="shared" si="1"/>
+        <v>221.40800000000002</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3">
+        <v>814</v>
+      </c>
+      <c r="E54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="4">
+        <f t="shared" si="1"/>
+        <v>3008.864</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3">
+        <v>11062</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change name exposures categories + correct error in naming of canton Geneva
</commit_message>
<xml_diff>
--- a/input_data/impact_functions/annual_deaths.xlsx
+++ b/input_data/impact_functions/annual_deaths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliestalhanske/python_projects/heat_mortality_impact/input_data/impact_functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A21EB70-7BD1-134D-A926-AD7A264C7E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BAB43E-55C4-ED4D-8E6D-100F119B08F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="19200" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Fribourg</t>
   </si>
   <si>
-    <t>Geneva</t>
-  </si>
-  <si>
     <t>Glarus</t>
   </si>
   <si>
@@ -131,10 +128,13 @@
     <t>annual_deaths</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>U</t>
+    <t>Over 75</t>
+  </si>
+  <si>
+    <t>Under 75</t>
+  </si>
+  <si>
+    <t>Genève</t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -501,24 +501,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2">
         <f>D2*C$2</f>
@@ -531,7 +531,7 @@
         <v>67088</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>4780</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>459</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -579,7 +579,7 @@
         <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>2446</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -611,7 +611,7 @@
         <v>2077</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -627,7 +627,7 @@
         <v>9451</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -643,12 +643,12 @@
         <v>2058</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
@@ -659,12 +659,12 @@
         <v>3385</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
@@ -675,12 +675,12 @@
         <v>363</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
@@ -691,12 +691,12 @@
         <v>1789</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
@@ -707,12 +707,12 @@
         <v>680</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
@@ -723,12 +723,12 @@
         <v>3140</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
@@ -739,12 +739,12 @@
         <v>1601</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
@@ -755,12 +755,12 @@
         <v>301</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
@@ -771,12 +771,12 @@
         <v>258</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
@@ -787,12 +787,12 @@
         <v>774</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
@@ -803,12 +803,12 @@
         <v>1152</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
@@ -819,12 +819,12 @@
         <v>2464</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="0"/>
@@ -835,12 +835,12 @@
         <v>3880</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
@@ -851,12 +851,12 @@
         <v>2067</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
@@ -867,12 +867,12 @@
         <v>3152</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
@@ -883,12 +883,12 @@
         <v>324</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
@@ -899,12 +899,12 @@
         <v>2724</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="0"/>
@@ -915,12 +915,12 @@
         <v>5750</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="0"/>
@@ -931,12 +931,12 @@
         <v>814</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="0"/>
@@ -947,12 +947,12 @@
         <v>11062</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="4">
         <f>D29*C$29</f>
@@ -965,7 +965,7 @@
         <v>67088</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -981,7 +981,7 @@
         <v>4780</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -997,7 +997,7 @@
         <v>459</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1013,7 +1013,7 @@
         <v>137</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>2446</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1045,7 +1045,7 @@
         <v>2077</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1061,7 +1061,7 @@
         <v>9451</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1077,12 +1077,12 @@
         <v>2058</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B37" s="4">
         <f t="shared" si="1"/>
@@ -1093,12 +1093,12 @@
         <v>3385</v>
       </c>
       <c r="E37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="4">
         <f t="shared" si="1"/>
@@ -1109,12 +1109,12 @@
         <v>363</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="4">
         <f t="shared" si="1"/>
@@ -1125,12 +1125,12 @@
         <v>1789</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="4">
         <f t="shared" si="1"/>
@@ -1141,12 +1141,12 @@
         <v>680</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="4">
         <f t="shared" si="1"/>
@@ -1157,12 +1157,12 @@
         <v>3140</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="4">
         <f t="shared" si="1"/>
@@ -1173,12 +1173,12 @@
         <v>1601</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B43" s="4">
         <f t="shared" si="1"/>
@@ -1189,12 +1189,12 @@
         <v>301</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44" s="4">
         <f t="shared" si="1"/>
@@ -1205,12 +1205,12 @@
         <v>258</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" s="4">
         <f t="shared" si="1"/>
@@ -1221,12 +1221,12 @@
         <v>774</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="4">
         <f t="shared" si="1"/>
@@ -1237,12 +1237,12 @@
         <v>1152</v>
       </c>
       <c r="E46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="4">
         <f t="shared" si="1"/>
@@ -1253,12 +1253,12 @@
         <v>2464</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" s="4">
         <f t="shared" si="1"/>
@@ -1269,12 +1269,12 @@
         <v>3880</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="4">
         <f t="shared" si="1"/>
@@ -1285,12 +1285,12 @@
         <v>2067</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="4">
         <f t="shared" si="1"/>
@@ -1301,12 +1301,12 @@
         <v>3152</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" s="4">
         <f t="shared" si="1"/>
@@ -1317,12 +1317,12 @@
         <v>324</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B52" s="4">
         <f t="shared" si="1"/>
@@ -1333,12 +1333,12 @@
         <v>2724</v>
       </c>
       <c r="E52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B53" s="4">
         <f t="shared" si="1"/>
@@ -1349,12 +1349,12 @@
         <v>5750</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B54" s="4">
         <f t="shared" si="1"/>
@@ -1365,12 +1365,12 @@
         <v>814</v>
       </c>
       <c r="E54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B55" s="4">
         <f t="shared" si="1"/>
@@ -1381,7 +1381,7 @@
         <v>11062</v>
       </c>
       <c r="E55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>